<commit_message>
Gannt diagram apparantly accepted.
</commit_message>
<xml_diff>
--- a/Excel_files/Gantt diagram.xlsx
+++ b/Excel_files/Gantt diagram.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">ACTIVITY</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">Final revision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It’s supposed to be like this, if there are no changes to make, we can copy paste the diagram</t>
   </si>
 </sst>
 </file>
@@ -74,6 +77,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -96,6 +100,7 @@
       <color rgb="FFA1467E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -103,12 +108,14 @@
       <color rgb="FF3465A4"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF3465A4"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -116,12 +123,14 @@
       <color rgb="FFF10D0C"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFF10D0C"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -259,7 +268,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -324,6 +333,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -340,12 +353,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -441,13 +458,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AL11"/>
+  <dimension ref="B1:AL14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="12.96"/>
@@ -671,11 +688,11 @@
         <v>5</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
       <c r="AL5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,11 +709,11 @@
         <v>5</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
       <c r="AL6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,15 +730,15 @@
         <v>5</v>
       </c>
       <c r="F7" s="12"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
       <c r="AL7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="7" t="n">
@@ -734,19 +751,19 @@
         <v>15</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="Z8" s="17"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="18"/>
-      <c r="AC8" s="18"/>
-      <c r="AD8" s="18"/>
-      <c r="AE8" s="17"/>
-      <c r="AF8" s="18"/>
-      <c r="AG8" s="18"/>
-      <c r="AH8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="19"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="19"/>
+      <c r="AG8" s="19"/>
+      <c r="AH8" s="19"/>
       <c r="AL8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="7" t="n">
@@ -759,15 +776,15 @@
         <v>5</v>
       </c>
       <c r="F9" s="12"/>
-      <c r="Z9" s="20"/>
-      <c r="AA9" s="20"/>
-      <c r="AB9" s="20"/>
-      <c r="AC9" s="20"/>
-      <c r="AD9" s="20"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="21"/>
+      <c r="AB9" s="21"/>
+      <c r="AC9" s="21"/>
+      <c r="AD9" s="21"/>
       <c r="AL9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7" t="n">
@@ -780,41 +797,41 @@
         <v>5</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="21"/>
-      <c r="AE10" s="17"/>
-      <c r="AF10" s="17"/>
-      <c r="AG10" s="17"/>
-      <c r="AH10" s="17"/>
-      <c r="AI10" s="21"/>
-      <c r="AJ10" s="21"/>
-      <c r="AK10" s="21"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="22"/>
+      <c r="AC10" s="22"/>
+      <c r="AD10" s="22"/>
+      <c r="AE10" s="23"/>
+      <c r="AF10" s="23"/>
+      <c r="AG10" s="23"/>
+      <c r="AH10" s="23"/>
+      <c r="AI10" s="22"/>
+      <c r="AJ10" s="22"/>
+      <c r="AK10" s="22"/>
       <c r="AL10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="7" t="n">
@@ -826,39 +843,44 @@
       <c r="E11" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-      <c r="S11" s="23"/>
-      <c r="T11" s="23"/>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="23"/>
-      <c r="AE11" s="23"/>
-      <c r="AF11" s="23"/>
-      <c r="AG11" s="23"/>
-      <c r="AH11" s="23"/>
-      <c r="AI11" s="24"/>
-      <c r="AJ11" s="24"/>
-      <c r="AK11" s="24"/>
-      <c r="AL11" s="25"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+      <c r="Y11" s="25"/>
+      <c r="Z11" s="25"/>
+      <c r="AA11" s="25"/>
+      <c r="AB11" s="25"/>
+      <c r="AC11" s="25"/>
+      <c r="AD11" s="25"/>
+      <c r="AE11" s="25"/>
+      <c r="AF11" s="25"/>
+      <c r="AG11" s="25"/>
+      <c r="AH11" s="25"/>
+      <c r="AI11" s="26"/>
+      <c r="AJ11" s="26"/>
+      <c r="AK11" s="26"/>
+      <c r="AL11" s="27"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>